<commit_message>
20200616 add 3 identity selection
</commit_message>
<xml_diff>
--- a/GUI_stdlist.xlsx
+++ b/GUI_stdlist.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Koach\Desktop\Office_guidace_System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\柯奇\py\office_guidance_sys\Office_Guidance_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA3DDF0-CAC6-499E-8C20-6B55D2F963DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8955" yWindow="2355" windowWidth="11385" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8955" yWindow="2355" windowWidth="11385" windowHeight="13245"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>std_num</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,11 +37,19 @@
     <t>ke</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>B123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -360,11 +367,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -388,6 +395,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>